<commit_message>
Updated 3D printed parts
</commit_message>
<xml_diff>
--- a/PartsFor20MicroRoversRev01.xlsx
+++ b/PartsFor20MicroRoversRev01.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nxt\Documents\GitHub\MicroRover\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdrk0011\Documents\GitHub\MicroRover\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
   <si>
     <t>Description</t>
   </si>
@@ -71,12 +71,6 @@
     <t>LPKF</t>
   </si>
   <si>
-    <t>3D Printing</t>
-  </si>
-  <si>
-    <t>Acrylic</t>
-  </si>
-  <si>
     <t>https://www.adafruit.com/product/2124</t>
   </si>
   <si>
@@ -125,9 +119,6 @@
     <t>Acklands Grainger</t>
   </si>
   <si>
-    <t>O-ring</t>
-  </si>
-  <si>
     <t>Johnson Industrial</t>
   </si>
   <si>
@@ -144,6 +135,30 @@
   </si>
   <si>
     <t>https://www.adafruit.com/product/598</t>
+  </si>
+  <si>
+    <t>Pololu</t>
+  </si>
+  <si>
+    <t>https://www.3dhubs.com/</t>
+  </si>
+  <si>
+    <t>3D Hubs</t>
+  </si>
+  <si>
+    <t>Rev02 prints without support</t>
+  </si>
+  <si>
+    <t>https://www.acklandsgrainger.com/en/product/O-RING-70BUNA-1X1-16/p/HBS568-022</t>
+  </si>
+  <si>
+    <t>O-ring BS1806-022</t>
+  </si>
+  <si>
+    <t>Estimate</t>
+  </si>
+  <si>
+    <t>Clear Acrylic 12"x24"</t>
   </si>
 </sst>
 </file>
@@ -151,7 +166,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -200,11 +215,11 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,66 +503,96 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="E4">
+        <v>40</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" ref="F4:F16" si="0">D4*E4</f>
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="E5">
+        <v>40</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -561,28 +606,36 @@
         <v>20</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" ref="F6:F16" si="0">D6*E6</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="D7" s="1">
+        <v>7.18</v>
+      </c>
       <c r="E7">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="F7" s="1">
         <f>D7*E7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+        <v>10.77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
         <v>37</v>
       </c>
       <c r="D8" s="1">
@@ -596,15 +649,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
         <v>26</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
       </c>
       <c r="D9" s="1">
         <v>1.95</v>
@@ -617,15 +670,15 @@
         <v>39</v>
       </c>
       <c r="G9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C10">
         <v>392</v>
@@ -641,18 +694,18 @@
         <v>4.95</v>
       </c>
       <c r="G10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C11">
         <v>598</v>
@@ -668,18 +721,18 @@
         <v>5.9</v>
       </c>
       <c r="G11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C12">
         <v>1500</v>
@@ -698,12 +751,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C13">
         <v>2124</v>
@@ -719,15 +772,15 @@
         <v>99</v>
       </c>
       <c r="G13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C14">
         <v>2442</v>
@@ -746,12 +799,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C15">
         <v>2750</v>
@@ -767,15 +820,15 @@
         <v>139</v>
       </c>
       <c r="G15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C16">
         <v>2892</v>
@@ -791,12 +844,12 @@
         <v>0.75</v>
       </c>
       <c r="G16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D17" s="1">
         <v>0.75</v>
@@ -809,22 +862,22 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F19" s="5">
         <f>SUM(F4:F17)</f>
-        <v>828.35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+        <v>857.12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F21" s="2">
         <f>F19/20</f>
-        <v>41.417500000000004</v>
+        <v>42.856000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added micro USB cable
</commit_message>
<xml_diff>
--- a/PartsFor20MicroRoversRev01.xlsx
+++ b/PartsFor20MicroRoversRev01.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
   <si>
     <t>Description</t>
   </si>
@@ -159,6 +159,15 @@
   </si>
   <si>
     <t>Clear Acrylic 12"x24"</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/592</t>
+  </si>
+  <si>
+    <t>Not sure about length yet</t>
+  </si>
+  <si>
+    <t>USB cable - A/MicroB - 3ft</t>
   </si>
 </sst>
 </file>
@@ -500,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,7 +570,7 @@
         <v>40</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" ref="F4:F16" si="0">D4*E4</f>
+        <f t="shared" ref="F4:F17" si="0">D4*E4</f>
         <v>12</v>
       </c>
       <c r="G4" t="s">
@@ -702,188 +711,215 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
         <v>28</v>
       </c>
       <c r="C11">
-        <v>598</v>
+        <v>592</v>
       </c>
       <c r="D11" s="1">
         <v>2.95</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" si="0"/>
-        <v>5.9</v>
+        <v>59</v>
       </c>
       <c r="G11" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="H11" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
         <v>28</v>
       </c>
       <c r="C12">
-        <v>1500</v>
+        <v>598</v>
       </c>
       <c r="D12" s="1">
-        <v>6.95</v>
+        <v>2.95</v>
       </c>
       <c r="E12">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" si="0"/>
-        <v>139</v>
+        <v>5.9</v>
       </c>
       <c r="G12" t="s">
-        <v>9</v>
+        <v>36</v>
+      </c>
+      <c r="H12" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
         <v>28</v>
       </c>
       <c r="C13">
-        <v>2124</v>
+        <v>1500</v>
       </c>
       <c r="D13" s="1">
-        <v>4.95</v>
+        <v>6.95</v>
       </c>
       <c r="E13">
         <v>20</v>
       </c>
       <c r="F13" s="1">
-        <f>D13*E13</f>
-        <v>99</v>
+        <f t="shared" si="0"/>
+        <v>139</v>
       </c>
       <c r="G13" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
         <v>28</v>
       </c>
       <c r="C14">
+        <v>2124</v>
+      </c>
+      <c r="D14" s="1">
+        <v>4.95</v>
+      </c>
+      <c r="E14">
+        <v>20</v>
+      </c>
+      <c r="F14" s="1">
+        <f>D14*E14</f>
+        <v>99</v>
+      </c>
+      <c r="G14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15">
         <v>2442</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D15" s="1">
         <v>7.5</v>
       </c>
-      <c r="E14">
+      <c r="E15">
         <v>40</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F15" s="1">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G15" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15">
-        <v>2750</v>
-      </c>
-      <c r="D15" s="1">
-        <v>6.95</v>
-      </c>
-      <c r="E15">
-        <v>20</v>
-      </c>
-      <c r="F15" s="1">
-        <f>D15*E15</f>
-        <v>139</v>
-      </c>
-      <c r="G15" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
         <v>28</v>
       </c>
       <c r="C16">
+        <v>2750</v>
+      </c>
+      <c r="D16" s="1">
+        <v>6.95</v>
+      </c>
+      <c r="E16">
+        <v>20</v>
+      </c>
+      <c r="F16" s="1">
+        <f>D16*E16</f>
+        <v>139</v>
+      </c>
+      <c r="G16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17">
         <v>2892</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D17" s="1">
         <v>0.75</v>
       </c>
-      <c r="E16">
+      <c r="E17">
         <v>1</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F17" s="1">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D18" s="1">
         <v>0.75</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <v>1</v>
       </c>
-      <c r="F17" s="1">
-        <f t="shared" ref="F17" si="1">D17*E17</f>
+      <c r="F18" s="1">
+        <f t="shared" ref="F18" si="1">D18*E18</f>
         <v>0.75</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="5">
-        <f>SUM(F4:F17)</f>
-        <v>857.12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="F20" s="5">
+        <f>SUM(F4:F18)</f>
+        <v>916.12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F21" s="2">
-        <f>F19/20</f>
-        <v>42.856000000000002</v>
+      <c r="F22" s="2">
+        <f>F20/20</f>
+        <v>45.805999999999997</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G12" r:id="rId1"/>
-    <hyperlink ref="G11" r:id="rId2"/>
+    <hyperlink ref="G13" r:id="rId1"/>
+    <hyperlink ref="G12" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
Starting to consider a group buy
</commit_message>
<xml_diff>
--- a/PartsFor20MicroRoversRev01.xlsx
+++ b/PartsFor20MicroRoversRev01.xlsx
@@ -512,6 +512,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -927,7 +930,8 @@
     <hyperlink ref="G13" r:id="rId1"/>
     <hyperlink ref="G12" r:id="rId2"/>
   </hyperlinks>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup scale="65" orientation="landscape" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>